<commit_message>
Add changes to gantt chart and gitignore
</commit_message>
<xml_diff>
--- a/1_Requirements/Gantt Chart.xlsx
+++ b/1_Requirements/Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D42FC1A-1621-4AE9-BC12-DBD985945A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46158806-41D5-473F-AEEC-2BDC556BA149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -243,9 +243,6 @@
     <t>Event Reminder (with Unit test)</t>
   </si>
   <si>
-    <t>Main  (with Unit test)</t>
-  </si>
-  <si>
     <t>MakeFile</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Clock App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main </t>
   </si>
 </sst>
 </file>
@@ -893,6 +893,18 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -900,18 +912,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1481,8 +1481,8 @@
   <dimension ref="A1:BL31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1504,7 +1504,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1533,118 +1533,118 @@
       <c r="B3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="87">
+      <c r="D3" s="86"/>
+      <c r="E3" s="84">
         <f>DATE(2021,6,23)</f>
         <v>44370</v>
       </c>
-      <c r="F3" s="87"/>
+      <c r="F3" s="84"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="84">
+      <c r="I4" s="81">
         <f>I5</f>
         <v>44368</v>
       </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="84">
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="81">
         <f>P5</f>
         <v>44375</v>
       </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="84">
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="81">
         <f>W5</f>
         <v>44382</v>
       </c>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="85"/>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="84">
+      <c r="X4" s="82"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="82"/>
+      <c r="AA4" s="82"/>
+      <c r="AB4" s="82"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="81">
         <f>AD5</f>
         <v>44389</v>
       </c>
-      <c r="AE4" s="85"/>
-      <c r="AF4" s="85"/>
-      <c r="AG4" s="85"/>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="85"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="84">
+      <c r="AE4" s="82"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="82"/>
+      <c r="AH4" s="82"/>
+      <c r="AI4" s="82"/>
+      <c r="AJ4" s="83"/>
+      <c r="AK4" s="81">
         <f>AK5</f>
         <v>44396</v>
       </c>
-      <c r="AL4" s="85"/>
-      <c r="AM4" s="85"/>
-      <c r="AN4" s="85"/>
-      <c r="AO4" s="85"/>
-      <c r="AP4" s="85"/>
-      <c r="AQ4" s="86"/>
-      <c r="AR4" s="84">
+      <c r="AL4" s="82"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="82"/>
+      <c r="AO4" s="82"/>
+      <c r="AP4" s="82"/>
+      <c r="AQ4" s="83"/>
+      <c r="AR4" s="81">
         <f>AR5</f>
         <v>44403</v>
       </c>
-      <c r="AS4" s="85"/>
-      <c r="AT4" s="85"/>
-      <c r="AU4" s="85"/>
-      <c r="AV4" s="85"/>
-      <c r="AW4" s="85"/>
-      <c r="AX4" s="86"/>
-      <c r="AY4" s="84">
+      <c r="AS4" s="82"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="82"/>
+      <c r="AV4" s="82"/>
+      <c r="AW4" s="82"/>
+      <c r="AX4" s="83"/>
+      <c r="AY4" s="81">
         <f>AY5</f>
         <v>44410</v>
       </c>
-      <c r="AZ4" s="85"/>
-      <c r="BA4" s="85"/>
-      <c r="BB4" s="85"/>
-      <c r="BC4" s="85"/>
-      <c r="BD4" s="85"/>
-      <c r="BE4" s="86"/>
-      <c r="BF4" s="84">
+      <c r="AZ4" s="82"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="82"/>
+      <c r="BC4" s="82"/>
+      <c r="BD4" s="82"/>
+      <c r="BE4" s="83"/>
+      <c r="BF4" s="81">
         <f>BF5</f>
         <v>44417</v>
       </c>
-      <c r="BG4" s="85"/>
-      <c r="BH4" s="85"/>
-      <c r="BI4" s="85"/>
-      <c r="BJ4" s="85"/>
-      <c r="BK4" s="85"/>
-      <c r="BL4" s="86"/>
+      <c r="BG4" s="82"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="82"/>
+      <c r="BJ4" s="82"/>
+      <c r="BK4" s="82"/>
+      <c r="BL4" s="83"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44368</v>
@@ -3146,7 +3146,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="31">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="67">
         <f>F19+1</f>
@@ -3461,7 +3461,9 @@
       <c r="C24" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="36"/>
+      <c r="D24" s="36">
+        <v>1</v>
+      </c>
       <c r="E24" s="68">
         <f>F23+1</f>
         <v>44384</v>
@@ -3535,12 +3537,14 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="57"/>
       <c r="B25" s="80" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C25" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="36"/>
+      <c r="D25" s="36">
+        <v>1</v>
+      </c>
       <c r="E25" s="68">
         <f>F24+1</f>
         <v>44386</v>
@@ -3614,7 +3618,7 @@
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="57"/>
       <c r="B26" s="80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="76" t="s">
         <v>43</v>
@@ -3695,7 +3699,7 @@
         <v>29</v>
       </c>
       <c r="B27" s="80" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="76" t="s">
         <v>43</v>
@@ -3856,6 +3860,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3863,11 +3872,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D28">
     <cfRule type="dataBar" priority="14">
@@ -4039,6 +4043,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EE49C3B21729434C834F03C10CFD3EE7" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dda2e0ad570191573d4862d24315b090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f90b35a-c7f5-466e-bdce-aad1192bcad3" xmlns:ns3="abad16e2-75b5-4d02-890c-30395bfef711" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="822e9fa36678c5abd975587ddd4d1967" ns2:_="" ns3:_="">
     <xsd:import namespace="3f90b35a-c7f5-466e-bdce-aad1192bcad3"/>
@@ -4249,22 +4268,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED231826-376F-4402-BA4A-6738EDB3C2A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCFEB13B-E464-42B4-95B6-1B297F6F0D89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A49C0C78-21B3-4F87-B703-D4DFD6AB582D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4281,21 +4302,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCFEB13B-E464-42B4-95B6-1B297F6F0D89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED231826-376F-4402-BA4A-6738EDB3C2A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>